<commit_message>
Added missing distances that were causing NA's after transformation
</commit_message>
<xml_diff>
--- a/Oyster_data/Quadrat/Grid_2013_2017/LCR_oyster_grid_2013_2017.xlsx
+++ b/Oyster_data/Quadrat/Grid_2013_2017/LCR_oyster_grid_2013_2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\billpine\Documents\GitHub\Data\Oyster_data\Quadrat\Grid_2013_2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevenbeck\Desktop\Reef_Project\Git\Data\Oyster_data\Quadrat\Grid_2013_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'grid data'!$B$1:$B$788</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -511,13 +511,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T788"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A758" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T786" sqref="T786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="13" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="2" customWidth="1"/>
@@ -23853,6 +23853,12 @@
       <c r="E652" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F652">
+        <v>0</v>
+      </c>
+      <c r="G652" s="2">
+        <v>2.8</v>
+      </c>
       <c r="H652">
         <v>27.7</v>
       </c>
@@ -23889,6 +23895,12 @@
       <c r="E653" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F653">
+        <v>0</v>
+      </c>
+      <c r="G653" s="2">
+        <v>2.8</v>
+      </c>
       <c r="H653">
         <v>11.3</v>
       </c>
@@ -23919,6 +23931,12 @@
       <c r="E654" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F654">
+        <v>11</v>
+      </c>
+      <c r="G654" s="2">
+        <v>1.8</v>
+      </c>
       <c r="H654">
         <v>0</v>
       </c>
@@ -23940,6 +23958,12 @@
       <c r="E655" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F655">
+        <v>4</v>
+      </c>
+      <c r="G655" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H655">
         <v>0</v>
       </c>
@@ -23961,6 +23985,12 @@
       <c r="E656" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F656">
+        <v>14</v>
+      </c>
+      <c r="G656" s="2">
+        <v>0.3</v>
+      </c>
       <c r="H656">
         <v>18.399999999999999</v>
       </c>
@@ -23991,6 +24021,12 @@
       <c r="E657" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F657">
+        <v>17</v>
+      </c>
+      <c r="G657" s="2">
+        <v>3.6</v>
+      </c>
       <c r="H657">
         <v>0</v>
       </c>
@@ -24012,6 +24048,12 @@
       <c r="E658" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F658">
+        <v>18</v>
+      </c>
+      <c r="G658" s="2">
+        <v>0.6</v>
+      </c>
       <c r="H658">
         <v>0</v>
       </c>
@@ -24033,6 +24075,12 @@
       <c r="E659" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F659">
+        <v>5</v>
+      </c>
+      <c r="G659" s="2">
+        <v>0</v>
+      </c>
       <c r="H659">
         <v>15.4</v>
       </c>
@@ -24054,6 +24102,12 @@
       <c r="E660" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F660">
+        <v>15</v>
+      </c>
+      <c r="G660" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H660">
         <v>0</v>
       </c>
@@ -24075,6 +24129,12 @@
       <c r="E661" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F661">
+        <v>6</v>
+      </c>
+      <c r="G661" s="2">
+        <v>3.3</v>
+      </c>
       <c r="H661">
         <v>12.8</v>
       </c>
@@ -24111,6 +24171,12 @@
       <c r="E662" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F662">
+        <v>6</v>
+      </c>
+      <c r="G662" s="2">
+        <v>3.3</v>
+      </c>
       <c r="H662">
         <v>12.4</v>
       </c>
@@ -24141,6 +24207,12 @@
       <c r="E663" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F663">
+        <v>13</v>
+      </c>
+      <c r="G663" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H663">
         <v>13.6</v>
       </c>
@@ -24182,6 +24254,12 @@
       <c r="E664" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F664">
+        <v>13</v>
+      </c>
+      <c r="G664" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H664">
         <v>19.8</v>
       </c>
@@ -24218,6 +24296,12 @@
       <c r="E665" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F665">
+        <v>13</v>
+      </c>
+      <c r="G665" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H665">
         <v>23.4</v>
       </c>
@@ -24254,6 +24338,12 @@
       <c r="E666" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F666">
+        <v>13</v>
+      </c>
+      <c r="G666" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H666">
         <v>21.9</v>
       </c>
@@ -24275,6 +24365,12 @@
       <c r="E667" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F667">
+        <v>18</v>
+      </c>
+      <c r="G667" s="2">
+        <v>1.4</v>
+      </c>
       <c r="H667">
         <v>0</v>
       </c>
@@ -24296,6 +24392,12 @@
       <c r="E668" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F668">
+        <v>17</v>
+      </c>
+      <c r="G668" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H668">
         <v>17.100000000000001</v>
       </c>
@@ -24338,6 +24440,12 @@
       <c r="E669" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F669">
+        <v>17</v>
+      </c>
+      <c r="G669" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H669">
         <v>18.2</v>
       </c>
@@ -24374,6 +24482,12 @@
       <c r="E670" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F670">
+        <v>17</v>
+      </c>
+      <c r="G670" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H670">
         <v>47.7</v>
       </c>
@@ -24410,6 +24524,12 @@
       <c r="E671" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F671">
+        <v>7</v>
+      </c>
+      <c r="G671" s="2">
+        <v>0.8</v>
+      </c>
       <c r="H671">
         <v>15.1</v>
       </c>
@@ -24445,6 +24565,12 @@
       <c r="E672" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F672">
+        <v>5</v>
+      </c>
+      <c r="G672" s="2">
+        <v>4</v>
+      </c>
       <c r="H672">
         <v>21.9</v>
       </c>
@@ -24481,6 +24607,12 @@
       <c r="E673" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F673">
+        <v>5</v>
+      </c>
+      <c r="G673" s="2">
+        <v>4</v>
+      </c>
       <c r="H673">
         <v>13.8</v>
       </c>
@@ -24505,6 +24637,12 @@
       <c r="E674" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F674">
+        <v>20</v>
+      </c>
+      <c r="G674" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H674">
         <v>23.7</v>
       </c>
@@ -24541,6 +24679,12 @@
       <c r="E675" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F675">
+        <v>20</v>
+      </c>
+      <c r="G675" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H675">
         <v>88.6</v>
       </c>
@@ -24568,6 +24712,12 @@
       <c r="E676" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F676">
+        <v>2</v>
+      </c>
+      <c r="G676" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H676">
         <v>43</v>
       </c>
@@ -24604,6 +24754,12 @@
       <c r="E677" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F677">
+        <v>2</v>
+      </c>
+      <c r="G677" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H677">
         <v>29.7</v>
       </c>
@@ -24634,6 +24790,12 @@
       <c r="E678" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F678">
+        <v>20</v>
+      </c>
+      <c r="G678" s="2">
+        <v>3.1</v>
+      </c>
       <c r="H678">
         <v>67.599999999999994</v>
       </c>
@@ -24676,6 +24838,12 @@
       <c r="E679" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F679">
+        <v>20</v>
+      </c>
+      <c r="G679" s="2">
+        <v>3.1</v>
+      </c>
       <c r="H679">
         <v>63.3</v>
       </c>
@@ -24703,6 +24871,12 @@
       <c r="E680" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F680">
+        <v>4</v>
+      </c>
+      <c r="G680" s="2">
+        <v>0.3</v>
+      </c>
       <c r="H680">
         <v>31.6</v>
       </c>
@@ -24744,6 +24918,12 @@
       <c r="E681" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F681">
+        <v>4</v>
+      </c>
+      <c r="G681" s="2">
+        <v>0.3</v>
+      </c>
       <c r="H681">
         <v>22.6</v>
       </c>
@@ -24771,6 +24951,12 @@
       <c r="E682" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F682">
+        <v>13</v>
+      </c>
+      <c r="G682" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H682">
         <v>35.700000000000003</v>
       </c>
@@ -24810,6 +24996,12 @@
       <c r="E683" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F683">
+        <v>13</v>
+      </c>
+      <c r="G683" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H683">
         <v>27.5</v>
       </c>
@@ -24837,6 +25029,12 @@
       <c r="E684" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F684">
+        <v>1</v>
+      </c>
+      <c r="G684" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H684">
         <v>15.3</v>
       </c>
@@ -24875,6 +25073,12 @@
       <c r="E685" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F685">
+        <v>0</v>
+      </c>
+      <c r="G685" s="2">
+        <v>0.8</v>
+      </c>
       <c r="H685">
         <v>33.200000000000003</v>
       </c>
@@ -24914,6 +25118,12 @@
       <c r="E686" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F686">
+        <v>1</v>
+      </c>
+      <c r="G686" s="2">
+        <v>4</v>
+      </c>
       <c r="H686">
         <v>59.5</v>
       </c>
@@ -24952,6 +25162,12 @@
       <c r="E687" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F687">
+        <v>1</v>
+      </c>
+      <c r="G687" s="2">
+        <v>4</v>
+      </c>
       <c r="H687">
         <v>40.299999999999997</v>
       </c>
@@ -24973,6 +25189,12 @@
       <c r="E688" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F688">
+        <v>19</v>
+      </c>
+      <c r="G688" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H688">
         <v>28.9</v>
       </c>
@@ -25015,6 +25237,12 @@
       <c r="E689" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F689">
+        <v>19</v>
+      </c>
+      <c r="G689" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H689">
         <v>40.200000000000003</v>
       </c>
@@ -25051,6 +25279,12 @@
       <c r="E690" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F690">
+        <v>19</v>
+      </c>
+      <c r="G690" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H690">
         <v>41.1</v>
       </c>
@@ -25087,6 +25321,12 @@
       <c r="E691" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F691">
+        <v>19</v>
+      </c>
+      <c r="G691" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H691">
         <v>24.3</v>
       </c>
@@ -25123,6 +25363,12 @@
       <c r="E692" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F692">
+        <v>1</v>
+      </c>
+      <c r="G692" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H692">
         <v>52.7</v>
       </c>
@@ -25165,6 +25411,12 @@
       <c r="E693" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F693">
+        <v>13</v>
+      </c>
+      <c r="G693" s="2">
+        <v>1.9</v>
+      </c>
       <c r="H693">
         <v>13.8</v>
       </c>
@@ -25201,6 +25453,12 @@
       <c r="E694" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F694">
+        <v>12</v>
+      </c>
+      <c r="G694" s="2">
+        <v>2.7</v>
+      </c>
       <c r="H694">
         <v>16.5</v>
       </c>
@@ -25240,6 +25498,12 @@
       <c r="E695" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F695">
+        <v>0</v>
+      </c>
+      <c r="G695" s="2">
+        <v>1.9</v>
+      </c>
       <c r="H695">
         <v>39.799999999999997</v>
       </c>
@@ -25269,6 +25533,12 @@
       <c r="E696" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F696">
+        <v>21</v>
+      </c>
+      <c r="G696" s="2">
+        <v>2</v>
+      </c>
       <c r="H696">
         <v>26.4</v>
       </c>
@@ -25311,6 +25581,12 @@
       <c r="E697" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F697">
+        <v>21</v>
+      </c>
+      <c r="G697" s="2">
+        <v>2</v>
+      </c>
       <c r="H697">
         <v>39.200000000000003</v>
       </c>
@@ -25347,6 +25623,12 @@
       <c r="E698" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F698">
+        <v>21</v>
+      </c>
+      <c r="G698" s="2">
+        <v>2</v>
+      </c>
       <c r="H698">
         <v>45.3</v>
       </c>
@@ -25374,6 +25656,12 @@
       <c r="E699" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F699">
+        <v>8</v>
+      </c>
+      <c r="G699" s="2">
+        <v>3.2</v>
+      </c>
       <c r="H699">
         <v>26.9</v>
       </c>
@@ -25412,6 +25700,12 @@
       <c r="E700" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F700">
+        <v>8</v>
+      </c>
+      <c r="G700" s="2">
+        <v>3.2</v>
+      </c>
       <c r="H700">
         <v>10.8</v>
       </c>
@@ -25439,6 +25733,12 @@
       <c r="E701" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F701">
+        <v>0</v>
+      </c>
+      <c r="G701" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H701">
         <v>29.5</v>
       </c>
@@ -25484,6 +25784,12 @@
       <c r="E702" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F702">
+        <v>0</v>
+      </c>
+      <c r="G702" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H702">
         <v>31.2</v>
       </c>
@@ -25517,6 +25823,12 @@
       <c r="E703" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F703">
+        <v>5</v>
+      </c>
+      <c r="G703" s="2">
+        <v>1.6</v>
+      </c>
       <c r="H703">
         <v>19.8</v>
       </c>
@@ -25553,6 +25865,12 @@
       <c r="E704" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F704">
+        <v>5</v>
+      </c>
+      <c r="G704" s="2">
+        <v>1.6</v>
+      </c>
       <c r="N704">
         <v>40.9</v>
       </c>
@@ -25583,6 +25901,12 @@
       <c r="E705" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F705">
+        <v>5</v>
+      </c>
+      <c r="G705" s="2">
+        <v>1.6</v>
+      </c>
       <c r="N705">
         <v>74.2</v>
       </c>
@@ -25607,6 +25931,12 @@
       <c r="E706" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F706">
+        <v>6</v>
+      </c>
+      <c r="G706" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H706">
         <v>22.8</v>
       </c>
@@ -25640,6 +25970,12 @@
       <c r="E707" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F707">
+        <v>5</v>
+      </c>
+      <c r="G707" s="2">
+        <v>2.8</v>
+      </c>
       <c r="H707">
         <v>19.8</v>
       </c>
@@ -25688,6 +26024,12 @@
       <c r="E708" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F708">
+        <v>5</v>
+      </c>
+      <c r="G708" s="2">
+        <v>2.8</v>
+      </c>
       <c r="N708">
         <v>11.5</v>
       </c>
@@ -25712,6 +26054,12 @@
       <c r="E709" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F709">
+        <v>2</v>
+      </c>
+      <c r="G709" s="2">
+        <v>3.8</v>
+      </c>
       <c r="H709">
         <v>15</v>
       </c>
@@ -25736,6 +26084,12 @@
       <c r="E710" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F710">
+        <v>9</v>
+      </c>
+      <c r="G710" s="2">
+        <v>1.8</v>
+      </c>
       <c r="H710">
         <v>61.4</v>
       </c>
@@ -25763,6 +26117,12 @@
       <c r="E711" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F711">
+        <v>10</v>
+      </c>
+      <c r="G711" s="2">
+        <v>0</v>
+      </c>
       <c r="N711">
         <v>62.7</v>
       </c>
@@ -25787,6 +26147,12 @@
       <c r="E712" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F712">
+        <v>5</v>
+      </c>
+      <c r="G712" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H712">
         <v>0</v>
       </c>
@@ -25808,6 +26174,12 @@
       <c r="E713" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F713">
+        <v>2</v>
+      </c>
+      <c r="G713" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H713">
         <v>0</v>
       </c>
@@ -25829,6 +26201,12 @@
       <c r="E714" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F714">
+        <v>20</v>
+      </c>
+      <c r="G714" s="2">
+        <v>1.9</v>
+      </c>
       <c r="H714">
         <v>13.5</v>
       </c>
@@ -25865,6 +26243,12 @@
       <c r="E715" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F715">
+        <v>12</v>
+      </c>
+      <c r="G715" s="2">
+        <v>1.4</v>
+      </c>
       <c r="H715">
         <v>20.8</v>
       </c>
@@ -25889,6 +26273,12 @@
       <c r="E716" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F716">
+        <v>21</v>
+      </c>
+      <c r="G716" s="2">
+        <v>3.9</v>
+      </c>
       <c r="H716">
         <v>23.5</v>
       </c>
@@ -25925,6 +26315,12 @@
       <c r="E717" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F717">
+        <v>13</v>
+      </c>
+      <c r="G717" s="2">
+        <v>2.5</v>
+      </c>
       <c r="H717">
         <v>19.100000000000001</v>
       </c>
@@ -25961,6 +26357,12 @@
       <c r="E718" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F718">
+        <v>13</v>
+      </c>
+      <c r="G718" s="2">
+        <v>2.5</v>
+      </c>
       <c r="H718">
         <v>85.3</v>
       </c>
@@ -25994,6 +26396,12 @@
       <c r="E719" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F719">
+        <v>18</v>
+      </c>
+      <c r="G719" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H719">
         <v>11.5</v>
       </c>
@@ -26023,6 +26431,12 @@
       <c r="E720" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F720">
+        <v>3</v>
+      </c>
+      <c r="G720" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H720">
         <v>16.100000000000001</v>
       </c>
@@ -26059,6 +26473,12 @@
       <c r="E721" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F721">
+        <v>3</v>
+      </c>
+      <c r="G721" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H721">
         <v>16</v>
       </c>
@@ -26095,6 +26515,12 @@
       <c r="E722" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F722">
+        <v>3</v>
+      </c>
+      <c r="G722" s="2">
+        <v>2.4</v>
+      </c>
       <c r="H722">
         <v>20.7</v>
       </c>
@@ -26131,6 +26557,12 @@
       <c r="E723" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F723">
+        <v>6</v>
+      </c>
+      <c r="G723" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H723">
         <v>19.399999999999999</v>
       </c>
@@ -26161,6 +26593,12 @@
       <c r="E724" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F724">
+        <v>17</v>
+      </c>
+      <c r="G724" s="2">
+        <v>3.6</v>
+      </c>
       <c r="H724">
         <v>16.2</v>
       </c>
@@ -26191,6 +26629,12 @@
       <c r="E725" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F725">
+        <v>5</v>
+      </c>
+      <c r="G725" s="2">
+        <v>3.1</v>
+      </c>
       <c r="H725">
         <v>15.3</v>
       </c>
@@ -26212,6 +26656,12 @@
       <c r="E726" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F726">
+        <v>4</v>
+      </c>
+      <c r="G726" s="2">
+        <v>1</v>
+      </c>
       <c r="H726">
         <v>27.6</v>
       </c>
@@ -26248,6 +26698,12 @@
       <c r="E727" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F727">
+        <v>4</v>
+      </c>
+      <c r="G727" s="2">
+        <v>1</v>
+      </c>
       <c r="H727">
         <v>20.3</v>
       </c>
@@ -26269,6 +26725,12 @@
       <c r="E728" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F728">
+        <v>18</v>
+      </c>
+      <c r="G728" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H728">
         <v>14.8</v>
       </c>
@@ -26305,6 +26767,12 @@
       <c r="E729" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F729">
+        <v>18</v>
+      </c>
+      <c r="G729" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H729">
         <v>14.9</v>
       </c>
@@ -26329,6 +26797,12 @@
       <c r="E730" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F730">
+        <v>9</v>
+      </c>
+      <c r="G730" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H730">
         <v>12.1</v>
       </c>
@@ -26365,6 +26839,12 @@
       <c r="E731" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F731">
+        <v>9</v>
+      </c>
+      <c r="G731" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H731">
         <v>15.2</v>
       </c>
@@ -26389,6 +26869,12 @@
       <c r="E732" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F732">
+        <v>4</v>
+      </c>
+      <c r="G732" s="2">
+        <v>4</v>
+      </c>
       <c r="H732">
         <v>14.6</v>
       </c>
@@ -26425,6 +26911,12 @@
       <c r="E733" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F733">
+        <v>18</v>
+      </c>
+      <c r="G733" s="2">
+        <v>1</v>
+      </c>
       <c r="H733">
         <v>13.6</v>
       </c>
@@ -26461,6 +26953,12 @@
       <c r="E734" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F734">
+        <v>18</v>
+      </c>
+      <c r="G734" s="2">
+        <v>1</v>
+      </c>
       <c r="H734">
         <v>8.9</v>
       </c>
@@ -26482,6 +26980,12 @@
       <c r="E735" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F735">
+        <v>5</v>
+      </c>
+      <c r="G735" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H735">
         <v>22.4</v>
       </c>
@@ -26521,6 +27025,12 @@
       <c r="E736" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F736">
+        <v>5</v>
+      </c>
+      <c r="G736" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H736">
         <v>14</v>
       </c>
@@ -26542,6 +27052,12 @@
       <c r="E737" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F737">
+        <v>18</v>
+      </c>
+      <c r="G737" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H737">
         <v>24.4</v>
       </c>
@@ -26578,6 +27094,12 @@
       <c r="E738" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F738">
+        <v>7</v>
+      </c>
+      <c r="G738" s="2">
+        <v>2.5</v>
+      </c>
       <c r="H738">
         <v>0</v>
       </c>
@@ -26599,6 +27121,12 @@
       <c r="E739" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F739">
+        <v>2</v>
+      </c>
+      <c r="G739" s="2">
+        <v>3.1</v>
+      </c>
       <c r="H739">
         <v>17.7</v>
       </c>
@@ -26626,6 +27154,12 @@
       <c r="E740" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F740">
+        <v>15</v>
+      </c>
+      <c r="G740" s="2">
+        <v>0.6</v>
+      </c>
       <c r="H740">
         <v>26.4</v>
       </c>
@@ -26664,6 +27198,12 @@
       <c r="E741" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F741">
+        <v>15</v>
+      </c>
+      <c r="G741" s="2">
+        <v>0.6</v>
+      </c>
       <c r="H741">
         <v>17.399999999999999</v>
       </c>
@@ -26685,6 +27225,12 @@
       <c r="E742" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F742">
+        <v>21</v>
+      </c>
+      <c r="G742" s="2">
+        <v>1</v>
+      </c>
       <c r="H742">
         <v>20</v>
       </c>
@@ -26718,6 +27264,12 @@
       <c r="E743" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F743">
+        <v>5</v>
+      </c>
+      <c r="G743" s="2">
+        <v>2.5</v>
+      </c>
       <c r="H743">
         <v>13.6</v>
       </c>
@@ -26748,6 +27300,12 @@
       <c r="E744" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F744">
+        <v>0</v>
+      </c>
+      <c r="G744" s="2">
+        <v>0.6</v>
+      </c>
       <c r="H744">
         <v>13.6</v>
       </c>
@@ -26777,6 +27335,12 @@
       <c r="E745" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F745">
+        <v>21</v>
+      </c>
+      <c r="G745" s="2">
+        <v>3.4</v>
+      </c>
       <c r="H745">
         <v>15.8</v>
       </c>
@@ -26800,6 +27364,12 @@
       <c r="E746" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F746">
+        <v>14</v>
+      </c>
+      <c r="G746" s="2">
+        <v>2</v>
+      </c>
       <c r="H746">
         <v>13.6</v>
       </c>
@@ -26824,6 +27394,12 @@
       <c r="E747" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F747">
+        <v>8</v>
+      </c>
+      <c r="G747" s="2">
+        <v>2.1</v>
+      </c>
       <c r="H747">
         <v>34</v>
       </c>
@@ -26860,6 +27436,12 @@
       <c r="E748" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F748">
+        <v>2</v>
+      </c>
+      <c r="G748" s="2">
+        <v>1</v>
+      </c>
       <c r="H748">
         <v>30.6</v>
       </c>
@@ -26896,6 +27478,12 @@
       <c r="E749" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F749">
+        <v>7</v>
+      </c>
+      <c r="G749" s="2">
+        <v>3</v>
+      </c>
       <c r="H749">
         <v>15.9</v>
       </c>
@@ -26934,6 +27522,12 @@
       <c r="E750" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F750">
+        <v>16</v>
+      </c>
+      <c r="G750" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H750">
         <v>14.6</v>
       </c>
@@ -26967,6 +27561,12 @@
       <c r="E751" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F751">
+        <v>2</v>
+      </c>
+      <c r="G751" s="2">
+        <v>0.4</v>
+      </c>
       <c r="H751">
         <v>13.6</v>
       </c>
@@ -26994,6 +27594,12 @@
       <c r="E752" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F752">
+        <v>4</v>
+      </c>
+      <c r="G752" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H752">
         <v>10.9</v>
       </c>
@@ -27030,6 +27636,12 @@
       <c r="E753" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F753">
+        <v>8</v>
+      </c>
+      <c r="G753" s="2">
+        <v>2.7</v>
+      </c>
       <c r="H753">
         <v>19.3</v>
       </c>
@@ -27069,6 +27681,12 @@
       <c r="E754" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F754">
+        <v>8</v>
+      </c>
+      <c r="G754" s="2">
+        <v>2.7</v>
+      </c>
       <c r="H754">
         <v>14.9</v>
       </c>
@@ -27096,6 +27714,12 @@
       <c r="E755" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F755">
+        <v>18</v>
+      </c>
+      <c r="G755" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H755">
         <v>17.899999999999999</v>
       </c>
@@ -27132,6 +27756,12 @@
       <c r="E756" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F756">
+        <v>0</v>
+      </c>
+      <c r="G756" s="2">
+        <v>3</v>
+      </c>
       <c r="H756">
         <v>85</v>
       </c>
@@ -27168,6 +27798,12 @@
       <c r="E757" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F757">
+        <v>0</v>
+      </c>
+      <c r="G757" s="2">
+        <v>3</v>
+      </c>
       <c r="H757">
         <v>21.5</v>
       </c>
@@ -27195,6 +27831,12 @@
       <c r="E758" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F758">
+        <v>16</v>
+      </c>
+      <c r="G758" s="2">
+        <v>2.8</v>
+      </c>
       <c r="H758">
         <v>11.5</v>
       </c>
@@ -27231,6 +27873,12 @@
       <c r="E759" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F759">
+        <v>16</v>
+      </c>
+      <c r="G759" s="2">
+        <v>2.8</v>
+      </c>
       <c r="H759">
         <v>14</v>
       </c>
@@ -27264,6 +27912,12 @@
       <c r="E760" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F760">
+        <v>14</v>
+      </c>
+      <c r="G760" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H760">
         <v>14.5</v>
       </c>
@@ -27300,6 +27954,12 @@
       <c r="E761" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F761">
+        <v>14</v>
+      </c>
+      <c r="G761" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="H761">
         <v>16.5</v>
       </c>
@@ -27330,6 +27990,12 @@
       <c r="E762" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F762">
+        <v>11</v>
+      </c>
+      <c r="G762" s="2">
+        <v>3.7</v>
+      </c>
       <c r="H762">
         <v>19</v>
       </c>
@@ -27351,6 +28017,12 @@
       <c r="E763" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F763">
+        <v>21</v>
+      </c>
+      <c r="G763" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H763">
         <v>26</v>
       </c>
@@ -27387,6 +28059,12 @@
       <c r="E764" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F764">
+        <v>21</v>
+      </c>
+      <c r="G764" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H764">
         <v>17</v>
       </c>
@@ -27408,6 +28086,12 @@
       <c r="E765" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F765">
+        <v>9</v>
+      </c>
+      <c r="G765" s="2">
+        <v>0.3</v>
+      </c>
       <c r="H765">
         <v>11.5</v>
       </c>
@@ -27441,6 +28125,12 @@
       <c r="E766" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F766">
+        <v>0</v>
+      </c>
+      <c r="G766" s="2">
+        <v>1.8</v>
+      </c>
       <c r="H766">
         <v>12.5</v>
       </c>
@@ -27479,6 +28169,12 @@
       <c r="E767" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F767">
+        <v>0</v>
+      </c>
+      <c r="G767" s="2">
+        <v>1.8</v>
+      </c>
       <c r="H767">
         <v>13</v>
       </c>
@@ -27500,6 +28196,12 @@
       <c r="E768" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F768">
+        <v>12</v>
+      </c>
+      <c r="G768" s="2">
+        <v>2.6</v>
+      </c>
       <c r="H768">
         <v>11.6</v>
       </c>
@@ -27521,6 +28223,12 @@
       <c r="E769" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F769">
+        <v>2</v>
+      </c>
+      <c r="G769" s="2">
+        <v>0.9</v>
+      </c>
       <c r="H769">
         <v>8.3000000000000007</v>
       </c>
@@ -27557,6 +28265,12 @@
       <c r="E770" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F770">
+        <v>2</v>
+      </c>
+      <c r="G770" s="2">
+        <v>0.9</v>
+      </c>
       <c r="H770">
         <v>13.1</v>
       </c>
@@ -27584,6 +28298,12 @@
       <c r="E771" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F771">
+        <v>11</v>
+      </c>
+      <c r="G771" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H771">
         <v>9.6</v>
       </c>
@@ -27623,6 +28343,12 @@
       <c r="E772" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F772">
+        <v>11</v>
+      </c>
+      <c r="G772" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H772">
         <v>25.9</v>
       </c>
@@ -27659,6 +28385,12 @@
       <c r="E773" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F773">
+        <v>11</v>
+      </c>
+      <c r="G773" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H773">
         <v>14.5</v>
       </c>
@@ -27695,6 +28427,12 @@
       <c r="E774" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F774">
+        <v>11</v>
+      </c>
+      <c r="G774" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H774">
         <v>20.100000000000001</v>
       </c>
@@ -27725,6 +28463,12 @@
       <c r="E775" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F775">
+        <v>13</v>
+      </c>
+      <c r="G775" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H775">
         <v>22.9</v>
       </c>
@@ -27769,6 +28513,12 @@
       <c r="E776" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F776">
+        <v>13</v>
+      </c>
+      <c r="G776" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H776">
         <v>8.5</v>
       </c>
@@ -27805,6 +28555,12 @@
       <c r="E777" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F777">
+        <v>13</v>
+      </c>
+      <c r="G777" s="2">
+        <v>0.7</v>
+      </c>
       <c r="H777">
         <v>18</v>
       </c>
@@ -27841,6 +28597,12 @@
       <c r="E778" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F778">
+        <v>3</v>
+      </c>
+      <c r="G778" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H778">
         <v>25</v>
       </c>
@@ -27877,6 +28639,12 @@
       <c r="E779" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F779">
+        <v>3</v>
+      </c>
+      <c r="G779" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H779">
         <v>18.7</v>
       </c>
@@ -27913,6 +28681,12 @@
       <c r="E780" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F780">
+        <v>3</v>
+      </c>
+      <c r="G780" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H780">
         <v>24.3</v>
       </c>
@@ -27949,6 +28723,12 @@
       <c r="E781" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F781">
+        <v>3</v>
+      </c>
+      <c r="G781" s="2">
+        <v>1.5</v>
+      </c>
       <c r="H781">
         <v>17.5</v>
       </c>
@@ -27973,6 +28753,12 @@
       <c r="E782" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F782">
+        <v>20</v>
+      </c>
+      <c r="G782" s="2">
+        <v>3.1</v>
+      </c>
       <c r="H782">
         <v>0</v>
       </c>
@@ -27994,6 +28780,12 @@
       <c r="E783" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F783">
+        <v>2</v>
+      </c>
+      <c r="G783" s="2">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="H783">
         <v>18.100000000000001</v>
       </c>
@@ -28027,6 +28819,12 @@
       <c r="E784" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F784">
+        <v>21</v>
+      </c>
+      <c r="G784" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H784">
         <v>13.1</v>
       </c>
@@ -28068,6 +28866,12 @@
       <c r="E785" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F785">
+        <v>21</v>
+      </c>
+      <c r="G785" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H785">
         <v>16.7</v>
       </c>
@@ -28104,6 +28908,12 @@
       <c r="E786" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F786">
+        <v>21</v>
+      </c>
+      <c r="G786" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H786">
         <v>6.6</v>
       </c>
@@ -28140,6 +28950,12 @@
       <c r="E787" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F787">
+        <v>21</v>
+      </c>
+      <c r="G787" s="2">
+        <v>1.3</v>
+      </c>
       <c r="H787">
         <v>12.6</v>
       </c>
@@ -28175,6 +28991,12 @@
       </c>
       <c r="E788" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="F788">
+        <v>21</v>
+      </c>
+      <c r="G788" s="2">
+        <v>1.3</v>
       </c>
       <c r="H788">
         <v>20</v>

</xml_diff>

<commit_message>
Addressed oyster quadrat data issues and added spreadsheet for spat collector data
</commit_message>
<xml_diff>
--- a/Oyster_data/Quadrat/Grid_2013_2017/LCR_oyster_grid_2013_2017.xlsx
+++ b/Oyster_data/Quadrat/Grid_2013_2017/LCR_oyster_grid_2013_2017.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2383" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2379" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -121,12 +121,6 @@
   </si>
   <si>
     <t>LCO1</t>
-  </si>
-  <si>
-    <t>1r</t>
-  </si>
-  <si>
-    <t>1L</t>
   </si>
   <si>
     <t>LCO5</t>
@@ -511,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A758" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T786" sqref="T786"/>
+    <sheetView tabSelected="1" topLeftCell="A287" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G313" sqref="G313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8912,6 +8906,9 @@
       <c r="F256">
         <v>8</v>
       </c>
+      <c r="G256" s="2">
+        <v>2.6</v>
+      </c>
       <c r="H256" s="3">
         <v>20.7</v>
       </c>
@@ -9020,6 +9017,9 @@
       <c r="F259">
         <v>8</v>
       </c>
+      <c r="G259" s="2">
+        <v>2.6</v>
+      </c>
       <c r="H259" s="3">
         <v>20.8</v>
       </c>
@@ -10863,8 +10863,8 @@
       <c r="F308">
         <v>6</v>
       </c>
-      <c r="G308" s="2" t="s">
-        <v>33</v>
+      <c r="G308" s="2">
+        <v>1</v>
       </c>
       <c r="H308" s="3">
         <v>18</v>
@@ -10904,8 +10904,8 @@
       <c r="F309">
         <v>6</v>
       </c>
-      <c r="G309" s="2" t="s">
-        <v>33</v>
+      <c r="G309" s="2">
+        <v>1</v>
       </c>
       <c r="H309" s="3">
         <v>35</v>
@@ -10945,8 +10945,8 @@
       <c r="F310">
         <v>6</v>
       </c>
-      <c r="G310" s="2" t="s">
-        <v>33</v>
+      <c r="G310" s="2">
+        <v>1</v>
       </c>
       <c r="H310" s="3">
         <v>25</v>
@@ -10986,8 +10986,8 @@
       <c r="F311">
         <v>6</v>
       </c>
-      <c r="G311" s="2" t="s">
-        <v>34</v>
+      <c r="G311" s="2">
+        <v>1</v>
       </c>
       <c r="H311">
         <v>22</v>
@@ -12306,7 +12306,7 @@
         <v>41940</v>
       </c>
       <c r="B345" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C345" s="2" t="s">
         <v>29</v>
@@ -12353,7 +12353,7 @@
         <v>41940</v>
       </c>
       <c r="B346" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>29</v>
@@ -12394,7 +12394,7 @@
         <v>41940</v>
       </c>
       <c r="B347" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C347" s="2" t="s">
         <v>29</v>
@@ -12417,7 +12417,7 @@
         <v>41940</v>
       </c>
       <c r="B348" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>29</v>
@@ -12440,7 +12440,7 @@
         <v>41940</v>
       </c>
       <c r="B349" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>29</v>
@@ -12481,7 +12481,7 @@
         <v>41940</v>
       </c>
       <c r="B350" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>29</v>
@@ -12522,7 +12522,7 @@
         <v>41940</v>
       </c>
       <c r="B351" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>29</v>
@@ -12563,7 +12563,7 @@
         <v>41940</v>
       </c>
       <c r="B352" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>29</v>
@@ -12604,7 +12604,7 @@
         <v>41940</v>
       </c>
       <c r="B353" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>29</v>
@@ -12645,7 +12645,7 @@
         <v>41940</v>
       </c>
       <c r="B354" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>29</v>
@@ -12686,7 +12686,7 @@
         <v>41940</v>
       </c>
       <c r="B355" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>29</v>
@@ -12727,7 +12727,7 @@
         <v>41940</v>
       </c>
       <c r="B356" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>29</v>
@@ -12768,7 +12768,7 @@
         <v>41940</v>
       </c>
       <c r="B357" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>29</v>
@@ -12797,7 +12797,7 @@
         <v>41940</v>
       </c>
       <c r="B358" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>29</v>
@@ -12826,7 +12826,7 @@
         <v>41940</v>
       </c>
       <c r="B359" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>29</v>
@@ -12867,7 +12867,7 @@
         <v>41940</v>
       </c>
       <c r="B360" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>29</v>
@@ -12908,7 +12908,7 @@
         <v>41940</v>
       </c>
       <c r="B361" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>29</v>
@@ -12949,7 +12949,7 @@
         <v>41940</v>
       </c>
       <c r="B362" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>29</v>
@@ -12990,7 +12990,7 @@
         <v>41940</v>
       </c>
       <c r="B363" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>29</v>
@@ -13025,7 +13025,7 @@
         <v>41940</v>
       </c>
       <c r="B364" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>29</v>
@@ -13070,7 +13070,7 @@
         <v>41940</v>
       </c>
       <c r="B365" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>29</v>
@@ -13099,7 +13099,7 @@
         <v>41940</v>
       </c>
       <c r="B366" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>29</v>
@@ -13140,7 +13140,7 @@
         <v>41940</v>
       </c>
       <c r="B367" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>29</v>
@@ -13181,7 +13181,7 @@
         <v>41940</v>
       </c>
       <c r="B368" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>29</v>
@@ -13222,7 +13222,7 @@
         <v>41940</v>
       </c>
       <c r="B369" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>29</v>
@@ -13263,7 +13263,7 @@
         <v>41940</v>
       </c>
       <c r="B370" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>29</v>
@@ -13298,7 +13298,7 @@
         <v>41940</v>
       </c>
       <c r="B371" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>29</v>
@@ -13339,7 +13339,7 @@
         <v>41940</v>
       </c>
       <c r="B372" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>29</v>
@@ -13380,7 +13380,7 @@
         <v>41940</v>
       </c>
       <c r="B373" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>29</v>
@@ -13421,7 +13421,7 @@
         <v>41940</v>
       </c>
       <c r="B374" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>29</v>
@@ -13450,7 +13450,7 @@
         <v>41940</v>
       </c>
       <c r="B375" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>29</v>
@@ -13491,7 +13491,7 @@
         <v>41940</v>
       </c>
       <c r="B376" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>29</v>
@@ -13532,7 +13532,7 @@
         <v>41940</v>
       </c>
       <c r="B377" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>29</v>
@@ -13576,7 +13576,7 @@
         <v>41940</v>
       </c>
       <c r="B378" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>29</v>
@@ -13620,7 +13620,7 @@
         <v>41940</v>
       </c>
       <c r="B379" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>29</v>
@@ -13661,7 +13661,7 @@
         <v>41940</v>
       </c>
       <c r="B380" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>29</v>
@@ -13702,7 +13702,7 @@
         <v>41940</v>
       </c>
       <c r="B381" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>29</v>
@@ -13731,7 +13731,7 @@
         <v>41940</v>
       </c>
       <c r="B382" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>29</v>
@@ -13772,7 +13772,7 @@
         <v>41940</v>
       </c>
       <c r="B383" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>29</v>
@@ -13813,7 +13813,7 @@
         <v>41940</v>
       </c>
       <c r="B384" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>29</v>
@@ -13845,7 +13845,7 @@
         <v>41940</v>
       </c>
       <c r="B385" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>29</v>
@@ -13868,7 +13868,7 @@
         <v>41940</v>
       </c>
       <c r="B386" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>29</v>
@@ -13912,7 +13912,7 @@
         <v>41940</v>
       </c>
       <c r="B387" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>29</v>
@@ -13947,7 +13947,7 @@
         <v>41940</v>
       </c>
       <c r="B388" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C388" s="2" t="s">
         <v>29</v>
@@ -13985,7 +13985,7 @@
         <v>41940</v>
       </c>
       <c r="B389" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>29</v>
@@ -14026,7 +14026,7 @@
         <v>41940</v>
       </c>
       <c r="B390" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>29</v>
@@ -14067,7 +14067,7 @@
         <v>41940</v>
       </c>
       <c r="B391" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>29</v>
@@ -14108,7 +14108,7 @@
         <v>41940</v>
       </c>
       <c r="B392" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>29</v>
@@ -14149,7 +14149,7 @@
         <v>41940</v>
       </c>
       <c r="B393" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>29</v>
@@ -14187,7 +14187,7 @@
         <v>41940</v>
       </c>
       <c r="B394" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>29</v>
@@ -14219,7 +14219,7 @@
         <v>41940</v>
       </c>
       <c r="B395" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>29</v>
@@ -14263,7 +14263,7 @@
         <v>41940</v>
       </c>
       <c r="B396" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>29</v>
@@ -14304,7 +14304,7 @@
         <v>41940</v>
       </c>
       <c r="B397" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>29</v>
@@ -14345,7 +14345,7 @@
         <v>41940</v>
       </c>
       <c r="B398" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>29</v>
@@ -14389,7 +14389,7 @@
         <v>41940</v>
       </c>
       <c r="B399" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>29</v>
@@ -14430,7 +14430,7 @@
         <v>41940</v>
       </c>
       <c r="B400" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>29</v>
@@ -14471,7 +14471,7 @@
         <v>41940</v>
       </c>
       <c r="B401" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C401" s="2" t="s">
         <v>29</v>
@@ -14512,7 +14512,7 @@
         <v>41940</v>
       </c>
       <c r="B402" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>29</v>
@@ -14551,7 +14551,7 @@
         <v>41940</v>
       </c>
       <c r="B403" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C403" s="2" t="s">
         <v>29</v>
@@ -14590,7 +14590,7 @@
         <v>41954</v>
       </c>
       <c r="B404" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>29</v>
@@ -14622,7 +14622,7 @@
         <v>41954</v>
       </c>
       <c r="B405" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C405" s="2" t="s">
         <v>29</v>
@@ -14657,7 +14657,7 @@
         <v>41954</v>
       </c>
       <c r="B406" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>29</v>
@@ -14698,7 +14698,7 @@
         <v>41954</v>
       </c>
       <c r="B407" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>29</v>
@@ -14739,7 +14739,7 @@
         <v>41954</v>
       </c>
       <c r="B408" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>29</v>
@@ -14783,7 +14783,7 @@
         <v>41954</v>
       </c>
       <c r="B409" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>29</v>
@@ -14812,7 +14812,7 @@
         <v>41954</v>
       </c>
       <c r="B410" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>29</v>
@@ -14844,7 +14844,7 @@
         <v>41954</v>
       </c>
       <c r="B411" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>29</v>
@@ -14882,7 +14882,7 @@
         <v>41954</v>
       </c>
       <c r="B412" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>29</v>
@@ -14923,7 +14923,7 @@
         <v>41954</v>
       </c>
       <c r="B413" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>29</v>
@@ -14964,7 +14964,7 @@
         <v>41954</v>
       </c>
       <c r="B414" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>29</v>
@@ -14999,7 +14999,7 @@
         <v>41954</v>
       </c>
       <c r="B415" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>29</v>
@@ -15043,7 +15043,7 @@
         <v>41954</v>
       </c>
       <c r="B416" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>29</v>
@@ -15084,7 +15084,7 @@
         <v>41954</v>
       </c>
       <c r="B417" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>29</v>
@@ -15125,7 +15125,7 @@
         <v>41954</v>
       </c>
       <c r="B418" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>29</v>
@@ -15166,7 +15166,7 @@
         <v>41954</v>
       </c>
       <c r="B419" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>29</v>
@@ -15213,7 +15213,7 @@
         <v>41954</v>
       </c>
       <c r="B420" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>29</v>
@@ -15254,7 +15254,7 @@
         <v>41954</v>
       </c>
       <c r="B421" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>29</v>
@@ -15295,7 +15295,7 @@
         <v>41954</v>
       </c>
       <c r="B422" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>29</v>
@@ -15336,7 +15336,7 @@
         <v>41954</v>
       </c>
       <c r="B423" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>29</v>
@@ -15377,7 +15377,7 @@
         <v>41954</v>
       </c>
       <c r="B424" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>29</v>
@@ -15406,7 +15406,7 @@
         <v>41954</v>
       </c>
       <c r="B425" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>29</v>
@@ -15447,7 +15447,7 @@
         <v>41954</v>
       </c>
       <c r="B426" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>29</v>
@@ -15491,7 +15491,7 @@
         <v>41954</v>
       </c>
       <c r="B427" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>29</v>
@@ -15532,7 +15532,7 @@
         <v>41954</v>
       </c>
       <c r="B428" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>29</v>
@@ -15564,7 +15564,7 @@
         <v>41954</v>
       </c>
       <c r="B429" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C429" s="2" t="s">
         <v>29</v>
@@ -15605,7 +15605,7 @@
         <v>41954</v>
       </c>
       <c r="B430" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>29</v>
@@ -15655,7 +15655,7 @@
         <v>41954</v>
       </c>
       <c r="B431" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>29</v>
@@ -15696,7 +15696,7 @@
         <v>41954</v>
       </c>
       <c r="B432" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>29</v>
@@ -15737,7 +15737,7 @@
         <v>41954</v>
       </c>
       <c r="B433" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>29</v>
@@ -16968,7 +16968,7 @@
         <v>41954</v>
       </c>
       <c r="B465" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>29</v>
@@ -17009,7 +17009,7 @@
         <v>41954</v>
       </c>
       <c r="B466" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>29</v>
@@ -17044,7 +17044,7 @@
         <v>41954</v>
       </c>
       <c r="B467" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C467" s="2" t="s">
         <v>29</v>
@@ -17070,7 +17070,7 @@
         <v>41954</v>
       </c>
       <c r="B468" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>29</v>
@@ -17114,7 +17114,7 @@
         <v>41954</v>
       </c>
       <c r="B469" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C469" s="2" t="s">
         <v>29</v>
@@ -17146,7 +17146,7 @@
         <v>41954</v>
       </c>
       <c r="B470" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>29</v>
@@ -17187,7 +17187,7 @@
         <v>41954</v>
       </c>
       <c r="B471" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>29</v>
@@ -17228,7 +17228,7 @@
         <v>41954</v>
       </c>
       <c r="B472" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>29</v>
@@ -17269,7 +17269,7 @@
         <v>41954</v>
       </c>
       <c r="B473" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>29</v>
@@ -17295,7 +17295,7 @@
         <v>41954</v>
       </c>
       <c r="B474" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C474" s="2" t="s">
         <v>29</v>
@@ -17327,7 +17327,7 @@
         <v>41954</v>
       </c>
       <c r="B475" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C475" s="2" t="s">
         <v>29</v>
@@ -17351,7 +17351,7 @@
         <v>41954</v>
       </c>
       <c r="B476" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C476" s="2" t="s">
         <v>29</v>
@@ -17392,7 +17392,7 @@
         <v>41954</v>
       </c>
       <c r="B477" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C477" s="2" t="s">
         <v>29</v>
@@ -17415,7 +17415,7 @@
         <v>41954</v>
       </c>
       <c r="B478" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C478" s="2" t="s">
         <v>29</v>
@@ -17450,7 +17450,7 @@
         <v>41954</v>
       </c>
       <c r="B479" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C479" s="2" t="s">
         <v>29</v>
@@ -17479,7 +17479,7 @@
         <v>41954</v>
       </c>
       <c r="B480" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C480" s="2" t="s">
         <v>29</v>
@@ -17511,7 +17511,7 @@
         <v>41954</v>
       </c>
       <c r="B481" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C481" s="2" t="s">
         <v>29</v>
@@ -17534,7 +17534,7 @@
         <v>41954</v>
       </c>
       <c r="B482" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C482" s="2" t="s">
         <v>29</v>
@@ -17563,7 +17563,7 @@
         <v>41954</v>
       </c>
       <c r="B483" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C483" s="2" t="s">
         <v>29</v>
@@ -17586,7 +17586,7 @@
         <v>41954</v>
       </c>
       <c r="B484" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C484" s="2" t="s">
         <v>29</v>
@@ -17627,7 +17627,7 @@
         <v>41954</v>
       </c>
       <c r="B485" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C485" s="2" t="s">
         <v>29</v>
@@ -17668,7 +17668,7 @@
         <v>41954</v>
       </c>
       <c r="B486" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C486" s="2" t="s">
         <v>29</v>
@@ -17694,7 +17694,7 @@
         <v>41954</v>
       </c>
       <c r="B487" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C487" s="2" t="s">
         <v>29</v>
@@ -17729,7 +17729,7 @@
         <v>41954</v>
       </c>
       <c r="B488" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C488" s="2" t="s">
         <v>29</v>
@@ -17755,7 +17755,7 @@
         <v>41954</v>
       </c>
       <c r="B489" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C489" s="2" t="s">
         <v>29</v>
@@ -17796,7 +17796,7 @@
         <v>41954</v>
       </c>
       <c r="B490" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C490" s="2" t="s">
         <v>29</v>
@@ -17819,7 +17819,7 @@
         <v>41954</v>
       </c>
       <c r="B491" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C491" s="2" t="s">
         <v>29</v>
@@ -17845,7 +17845,7 @@
         <v>41954</v>
       </c>
       <c r="B492" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C492" s="2" t="s">
         <v>29</v>
@@ -17886,7 +17886,7 @@
         <v>41954</v>
       </c>
       <c r="B493" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C493" s="2" t="s">
         <v>29</v>
@@ -17909,7 +17909,7 @@
         <v>41954</v>
       </c>
       <c r="B494" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C494" s="2" t="s">
         <v>29</v>
@@ -17950,7 +17950,7 @@
         <v>41954</v>
       </c>
       <c r="B495" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C495" s="2" t="s">
         <v>29</v>
@@ -17988,7 +17988,7 @@
         <v>41954</v>
       </c>
       <c r="B496" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C496" s="2" t="s">
         <v>29</v>
@@ -18017,7 +18017,7 @@
         <v>41954</v>
       </c>
       <c r="B497" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C497" s="2" t="s">
         <v>29</v>
@@ -18040,7 +18040,7 @@
         <v>41954</v>
       </c>
       <c r="B498" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C498" s="2" t="s">
         <v>29</v>
@@ -18072,7 +18072,7 @@
         <v>41954</v>
       </c>
       <c r="B499" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C499" s="2" t="s">
         <v>29</v>
@@ -18101,7 +18101,7 @@
         <v>41954</v>
       </c>
       <c r="B500" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C500" s="2" t="s">
         <v>29</v>
@@ -18127,7 +18127,7 @@
         <v>41954</v>
       </c>
       <c r="B501" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C501" s="2" t="s">
         <v>29</v>
@@ -18150,7 +18150,7 @@
         <v>41954</v>
       </c>
       <c r="B502" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C502" s="2" t="s">
         <v>29</v>
@@ -18185,7 +18185,7 @@
         <v>41954</v>
       </c>
       <c r="B503" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C503" s="2" t="s">
         <v>29</v>
@@ -18214,7 +18214,7 @@
         <v>41954</v>
       </c>
       <c r="B504" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C504" s="2" t="s">
         <v>29</v>
@@ -18240,7 +18240,7 @@
         <v>41954</v>
       </c>
       <c r="B505" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C505" s="2" t="s">
         <v>29</v>
@@ -18272,7 +18272,7 @@
         <v>41954</v>
       </c>
       <c r="B506" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C506" s="2" t="s">
         <v>29</v>
@@ -18295,7 +18295,7 @@
         <v>41954</v>
       </c>
       <c r="B507" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C507" s="2" t="s">
         <v>29</v>
@@ -18336,7 +18336,7 @@
         <v>41954</v>
       </c>
       <c r="B508" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C508" s="2" t="s">
         <v>29</v>
@@ -18359,7 +18359,7 @@
         <v>41954</v>
       </c>
       <c r="B509" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C509" s="2" t="s">
         <v>29</v>
@@ -18382,7 +18382,7 @@
         <v>41954</v>
       </c>
       <c r="B510" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C510" s="2" t="s">
         <v>29</v>
@@ -18423,7 +18423,7 @@
         <v>41954</v>
       </c>
       <c r="B511" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C511" s="2" t="s">
         <v>29</v>
@@ -18447,7 +18447,7 @@
         <v>41954</v>
       </c>
       <c r="B512" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C512" s="2" t="s">
         <v>29</v>
@@ -18470,7 +18470,7 @@
         <v>41954</v>
       </c>
       <c r="B513" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C513" s="2" t="s">
         <v>29</v>
@@ -18493,7 +18493,7 @@
         <v>41954</v>
       </c>
       <c r="B514" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C514" s="2" t="s">
         <v>29</v>
@@ -18516,7 +18516,7 @@
         <v>41954</v>
       </c>
       <c r="B515" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C515" s="2" t="s">
         <v>29</v>
@@ -18539,7 +18539,7 @@
         <v>41954</v>
       </c>
       <c r="B516" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C516" s="2" t="s">
         <v>29</v>
@@ -18562,7 +18562,7 @@
         <v>41978</v>
       </c>
       <c r="B517" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C517" s="2" t="s">
         <v>29</v>
@@ -18603,7 +18603,7 @@
         <v>41978</v>
       </c>
       <c r="B518" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C518" s="2" t="s">
         <v>29</v>
@@ -18629,7 +18629,7 @@
         <v>41978</v>
       </c>
       <c r="B519" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C519" s="2" t="s">
         <v>29</v>
@@ -18670,7 +18670,7 @@
         <v>41978</v>
       </c>
       <c r="B520" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C520" s="2" t="s">
         <v>29</v>
@@ -18711,7 +18711,7 @@
         <v>41978</v>
       </c>
       <c r="B521" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C521" s="2" t="s">
         <v>29</v>
@@ -18743,7 +18743,7 @@
         <v>41978</v>
       </c>
       <c r="B522" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C522" s="2" t="s">
         <v>29</v>
@@ -18784,7 +18784,7 @@
         <v>41978</v>
       </c>
       <c r="B523" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C523" s="2" t="s">
         <v>29</v>
@@ -18816,7 +18816,7 @@
         <v>41978</v>
       </c>
       <c r="B524" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C524" s="2" t="s">
         <v>29</v>
@@ -18842,7 +18842,7 @@
         <v>41978</v>
       </c>
       <c r="B525" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C525" s="2" t="s">
         <v>29</v>
@@ -18865,7 +18865,7 @@
         <v>41978</v>
       </c>
       <c r="B526" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C526" s="2" t="s">
         <v>29</v>
@@ -18906,7 +18906,7 @@
         <v>41978</v>
       </c>
       <c r="B527" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C527" s="2" t="s">
         <v>29</v>
@@ -18947,7 +18947,7 @@
         <v>41978</v>
       </c>
       <c r="B528" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C528" s="2" t="s">
         <v>29</v>
@@ -18973,7 +18973,7 @@
         <v>41978</v>
       </c>
       <c r="B529" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C529" s="2" t="s">
         <v>29</v>
@@ -19017,7 +19017,7 @@
         <v>32</v>
       </c>
       <c r="C530" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D530" s="2">
         <v>1</v>
@@ -19053,7 +19053,7 @@
         <v>32</v>
       </c>
       <c r="C531" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D531" s="2">
         <v>1</v>
@@ -19098,7 +19098,7 @@
         <v>32</v>
       </c>
       <c r="C532" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D532" s="2">
         <v>1</v>
@@ -19143,7 +19143,7 @@
         <v>32</v>
       </c>
       <c r="C533" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D533" s="2">
         <v>1</v>
@@ -19172,7 +19172,7 @@
         <v>32</v>
       </c>
       <c r="C534" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D534" s="2">
         <v>1</v>
@@ -19217,7 +19217,7 @@
         <v>32</v>
       </c>
       <c r="C535" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D535" s="2">
         <v>1</v>
@@ -19259,7 +19259,7 @@
         <v>32</v>
       </c>
       <c r="C536" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D536" s="2">
         <v>1</v>
@@ -19298,7 +19298,7 @@
         <v>32</v>
       </c>
       <c r="C537" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D537" s="2">
         <v>1</v>
@@ -19327,7 +19327,7 @@
         <v>32</v>
       </c>
       <c r="C538" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D538" s="2">
         <v>1</v>
@@ -19377,7 +19377,7 @@
         <v>32</v>
       </c>
       <c r="C539" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D539" s="2">
         <v>1</v>
@@ -19416,7 +19416,7 @@
         <v>32</v>
       </c>
       <c r="C540" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D540" s="2">
         <v>2</v>
@@ -19461,7 +19461,7 @@
         <v>32</v>
       </c>
       <c r="C541" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D541" s="2">
         <v>2</v>
@@ -19505,7 +19505,7 @@
         <v>32</v>
       </c>
       <c r="C542" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D542" s="2">
         <v>2</v>
@@ -19547,7 +19547,7 @@
         <v>32</v>
       </c>
       <c r="C543" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D543" s="2">
         <v>2</v>
@@ -19589,7 +19589,7 @@
         <v>32</v>
       </c>
       <c r="C544" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D544" s="2">
         <v>2</v>
@@ -19628,7 +19628,7 @@
         <v>32</v>
       </c>
       <c r="C545" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D545" s="2">
         <v>2</v>
@@ -19673,7 +19673,7 @@
         <v>32</v>
       </c>
       <c r="C546" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D546" s="2">
         <v>2</v>
@@ -19712,7 +19712,7 @@
         <v>32</v>
       </c>
       <c r="C547" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D547" s="2">
         <v>2</v>
@@ -19754,7 +19754,7 @@
         <v>32</v>
       </c>
       <c r="C548" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D548" s="2">
         <v>2</v>
@@ -19789,7 +19789,7 @@
         <v>32</v>
       </c>
       <c r="C549" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D549" s="2">
         <v>3</v>
@@ -19840,7 +19840,7 @@
         <v>32</v>
       </c>
       <c r="C550" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D550" s="2">
         <v>3</v>
@@ -19876,7 +19876,7 @@
         <v>32</v>
       </c>
       <c r="C551" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D551" s="2">
         <v>3</v>
@@ -19912,7 +19912,7 @@
         <v>32</v>
       </c>
       <c r="C552" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D552" s="2">
         <v>3</v>
@@ -19954,7 +19954,7 @@
         <v>32</v>
       </c>
       <c r="C553" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D553" s="2">
         <v>3</v>
@@ -19993,7 +19993,7 @@
         <v>32</v>
       </c>
       <c r="C554" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D554" s="2">
         <v>3</v>
@@ -20040,7 +20040,7 @@
         <v>32</v>
       </c>
       <c r="C555" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D555" s="2">
         <v>3</v>
@@ -20067,7 +20067,7 @@
         <v>32</v>
       </c>
       <c r="C556" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D556" s="2">
         <v>3</v>
@@ -20117,7 +20117,7 @@
         <v>32</v>
       </c>
       <c r="C557" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D557" s="2">
         <v>3</v>
@@ -20159,7 +20159,7 @@
         <v>32</v>
       </c>
       <c r="C558" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D558" s="2">
         <v>3</v>
@@ -20195,7 +20195,7 @@
         <v>28</v>
       </c>
       <c r="C559" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D559" s="2">
         <v>1</v>
@@ -20239,7 +20239,7 @@
         <v>28</v>
       </c>
       <c r="C560" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D560" s="2">
         <v>1</v>
@@ -20281,7 +20281,7 @@
         <v>28</v>
       </c>
       <c r="C561" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D561" s="2">
         <v>1</v>
@@ -20323,7 +20323,7 @@
         <v>28</v>
       </c>
       <c r="C562" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D562" s="2">
         <v>1</v>
@@ -20376,7 +20376,7 @@
         <v>28</v>
       </c>
       <c r="C563" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D563" s="2">
         <v>1</v>
@@ -20418,7 +20418,7 @@
         <v>28</v>
       </c>
       <c r="C564" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D564" s="2">
         <v>1</v>
@@ -20457,7 +20457,7 @@
         <v>28</v>
       </c>
       <c r="C565" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D565" s="2">
         <v>1</v>
@@ -20501,7 +20501,7 @@
         <v>28</v>
       </c>
       <c r="C566" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D566" s="2">
         <v>1</v>
@@ -20543,7 +20543,7 @@
         <v>28</v>
       </c>
       <c r="C567" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D567" s="2">
         <v>2</v>
@@ -20590,7 +20590,7 @@
         <v>28</v>
       </c>
       <c r="C568" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D568" s="2">
         <v>2</v>
@@ -20632,7 +20632,7 @@
         <v>28</v>
       </c>
       <c r="C569" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D569" s="2">
         <v>2</v>
@@ -20674,7 +20674,7 @@
         <v>28</v>
       </c>
       <c r="C570" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D570" s="2">
         <v>2</v>
@@ -20716,7 +20716,7 @@
         <v>28</v>
       </c>
       <c r="C571" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D571" s="2">
         <v>2</v>
@@ -20758,7 +20758,7 @@
         <v>28</v>
       </c>
       <c r="C572" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D572" s="2">
         <v>2</v>
@@ -20794,7 +20794,7 @@
         <v>28</v>
       </c>
       <c r="C573" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D573" s="2">
         <v>2</v>
@@ -20836,7 +20836,7 @@
         <v>28</v>
       </c>
       <c r="C574" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D574" s="2">
         <v>2</v>
@@ -20872,7 +20872,7 @@
         <v>28</v>
       </c>
       <c r="C575" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D575" s="2">
         <v>2</v>
@@ -20913,7 +20913,7 @@
         <v>28</v>
       </c>
       <c r="C576" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D576" s="2">
         <v>3</v>
@@ -20964,7 +20964,7 @@
         <v>28</v>
       </c>
       <c r="C577" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D577" s="2">
         <v>3</v>
@@ -21000,7 +21000,7 @@
         <v>28</v>
       </c>
       <c r="C578" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D578" s="2">
         <v>3</v>
@@ -21048,7 +21048,7 @@
         <v>28</v>
       </c>
       <c r="C579" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D579" s="2">
         <v>3</v>
@@ -21090,7 +21090,7 @@
         <v>28</v>
       </c>
       <c r="C580" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D580" s="2">
         <v>3</v>
@@ -21132,7 +21132,7 @@
         <v>28</v>
       </c>
       <c r="C581" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D581" s="2">
         <v>3</v>
@@ -21174,7 +21174,7 @@
         <v>28</v>
       </c>
       <c r="C582" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D582" s="2">
         <v>3</v>
@@ -21219,7 +21219,7 @@
         <v>28</v>
       </c>
       <c r="C583" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D583" s="2">
         <v>3</v>
@@ -21257,7 +21257,7 @@
         <v>31</v>
       </c>
       <c r="C584" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D584" s="2">
         <v>1</v>
@@ -21299,7 +21299,7 @@
         <v>31</v>
       </c>
       <c r="C585" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D585" s="2">
         <v>1</v>
@@ -21341,7 +21341,7 @@
         <v>31</v>
       </c>
       <c r="C586" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D586" s="2">
         <v>1</v>
@@ -21371,7 +21371,7 @@
         <v>31</v>
       </c>
       <c r="C587" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D587" s="2">
         <v>1</v>
@@ -21415,7 +21415,7 @@
         <v>31</v>
       </c>
       <c r="C588" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D588" s="2">
         <v>1</v>
@@ -21445,7 +21445,7 @@
         <v>31</v>
       </c>
       <c r="C589" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D589" s="2">
         <v>1</v>
@@ -21484,7 +21484,7 @@
         <v>31</v>
       </c>
       <c r="C590" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D590" s="2">
         <v>1</v>
@@ -21526,7 +21526,7 @@
         <v>31</v>
       </c>
       <c r="C591" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D591" s="2">
         <v>1</v>
@@ -21559,7 +21559,7 @@
         <v>31</v>
       </c>
       <c r="C592" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D592" s="2">
         <v>1</v>
@@ -21601,7 +21601,7 @@
         <v>31</v>
       </c>
       <c r="C593" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D593" s="2">
         <v>1</v>
@@ -21631,7 +21631,7 @@
         <v>31</v>
       </c>
       <c r="C594" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D594" s="2">
         <v>1</v>
@@ -21675,7 +21675,7 @@
         <v>31</v>
       </c>
       <c r="C595" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D595" s="2">
         <v>2</v>
@@ -21717,7 +21717,7 @@
         <v>31</v>
       </c>
       <c r="C596" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D596" s="2">
         <v>2</v>
@@ -21747,7 +21747,7 @@
         <v>31</v>
       </c>
       <c r="C597" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D597" s="2">
         <v>2</v>
@@ -21789,7 +21789,7 @@
         <v>31</v>
       </c>
       <c r="C598" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D598" s="2">
         <v>2</v>
@@ -21819,7 +21819,7 @@
         <v>31</v>
       </c>
       <c r="C599" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D599" s="2">
         <v>2</v>
@@ -21857,7 +21857,7 @@
         <v>31</v>
       </c>
       <c r="C600" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D600" s="2">
         <v>2</v>
@@ -21899,7 +21899,7 @@
         <v>31</v>
       </c>
       <c r="C601" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D601" s="2">
         <v>2</v>
@@ -21941,7 +21941,7 @@
         <v>31</v>
       </c>
       <c r="C602" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D602" s="2">
         <v>2</v>
@@ -21985,7 +21985,7 @@
         <v>31</v>
       </c>
       <c r="C603" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D603" s="2">
         <v>2</v>
@@ -22030,7 +22030,7 @@
         <v>31</v>
       </c>
       <c r="C604" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D604" s="2">
         <v>2</v>
@@ -22069,7 +22069,7 @@
         <v>31</v>
       </c>
       <c r="C605" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D605" s="2">
         <v>3</v>
@@ -22117,7 +22117,7 @@
         <v>31</v>
       </c>
       <c r="C606" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D606" s="2">
         <v>3</v>
@@ -22159,7 +22159,7 @@
         <v>31</v>
       </c>
       <c r="C607" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D607" s="2">
         <v>3</v>
@@ -22201,7 +22201,7 @@
         <v>31</v>
       </c>
       <c r="C608" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D608" s="2">
         <v>3</v>
@@ -22240,7 +22240,7 @@
         <v>31</v>
       </c>
       <c r="C609" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D609" s="2">
         <v>3</v>
@@ -22281,7 +22281,7 @@
         <v>31</v>
       </c>
       <c r="C610" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D610" s="2">
         <v>3</v>
@@ -22320,7 +22320,7 @@
         <v>31</v>
       </c>
       <c r="C611" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D611" s="2">
         <v>3</v>
@@ -22365,7 +22365,7 @@
         <v>31</v>
       </c>
       <c r="C612" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D612" s="2">
         <v>3</v>
@@ -22407,7 +22407,7 @@
         <v>31</v>
       </c>
       <c r="C613" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D613" s="2">
         <v>3</v>
@@ -22434,7 +22434,7 @@
         <v>31</v>
       </c>
       <c r="C614" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D614" s="2">
         <v>3</v>
@@ -22473,7 +22473,7 @@
         <v>31</v>
       </c>
       <c r="C615" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D615" s="2">
         <v>3</v>
@@ -22497,10 +22497,10 @@
         <v>43047</v>
       </c>
       <c r="B616" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C616" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D616" s="2">
         <v>1</v>
@@ -22539,10 +22539,10 @@
         <v>43047</v>
       </c>
       <c r="B617" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C617" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D617" s="2">
         <v>1</v>
@@ -22572,10 +22572,10 @@
         <v>43047</v>
       </c>
       <c r="B618" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C618" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D618" s="2">
         <v>1</v>
@@ -22614,10 +22614,10 @@
         <v>43047</v>
       </c>
       <c r="B619" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C619" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D619" s="2">
         <v>1</v>
@@ -22644,10 +22644,10 @@
         <v>43047</v>
       </c>
       <c r="B620" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C620" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D620" s="2">
         <v>1</v>
@@ -22686,10 +22686,10 @@
         <v>43047</v>
       </c>
       <c r="B621" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C621" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D621" s="2">
         <v>1</v>
@@ -22719,10 +22719,10 @@
         <v>43047</v>
       </c>
       <c r="B622" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C622" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D622" s="2">
         <v>1</v>
@@ -22763,10 +22763,10 @@
         <v>43047</v>
       </c>
       <c r="B623" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C623" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D623" s="2">
         <v>1</v>
@@ -22802,10 +22802,10 @@
         <v>43047</v>
       </c>
       <c r="B624" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C624" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D624" s="2">
         <v>1</v>
@@ -22847,10 +22847,10 @@
         <v>43047</v>
       </c>
       <c r="B625" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C625" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D625" s="2">
         <v>1</v>
@@ -22877,10 +22877,10 @@
         <v>43047</v>
       </c>
       <c r="B626" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C626" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D626" s="2">
         <v>1</v>
@@ -22915,10 +22915,10 @@
         <v>43047</v>
       </c>
       <c r="B627" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C627" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D627" s="2">
         <v>2</v>
@@ -22948,10 +22948,10 @@
         <v>43047</v>
       </c>
       <c r="B628" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C628" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D628" s="2">
         <v>2</v>
@@ -22981,10 +22981,10 @@
         <v>43047</v>
       </c>
       <c r="B629" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C629" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D629" s="2">
         <v>2</v>
@@ -23023,10 +23023,10 @@
         <v>43047</v>
       </c>
       <c r="B630" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C630" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D630" s="2">
         <v>2</v>
@@ -23053,10 +23053,10 @@
         <v>43047</v>
       </c>
       <c r="B631" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C631" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D631" s="2">
         <v>2</v>
@@ -23098,10 +23098,10 @@
         <v>43047</v>
       </c>
       <c r="B632" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C632" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D632" s="2">
         <v>2</v>
@@ -23125,10 +23125,10 @@
         <v>43047</v>
       </c>
       <c r="B633" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C633" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D633" s="2">
         <v>2</v>
@@ -23167,10 +23167,10 @@
         <v>43047</v>
       </c>
       <c r="B634" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C634" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D634" s="2">
         <v>2</v>
@@ -23197,10 +23197,10 @@
         <v>43047</v>
       </c>
       <c r="B635" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C635" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D635" s="2">
         <v>2</v>
@@ -23245,10 +23245,10 @@
         <v>43047</v>
       </c>
       <c r="B636" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C636" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D636" s="2">
         <v>2</v>
@@ -23284,10 +23284,10 @@
         <v>43047</v>
       </c>
       <c r="B637" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C637" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D637" s="2">
         <v>2</v>
@@ -23311,10 +23311,10 @@
         <v>43047</v>
       </c>
       <c r="B638" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C638" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D638" s="2">
         <v>2</v>
@@ -23350,10 +23350,10 @@
         <v>43047</v>
       </c>
       <c r="B639" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C639" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D639" s="2">
         <v>2</v>
@@ -23377,10 +23377,10 @@
         <v>43047</v>
       </c>
       <c r="B640" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C640" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D640" s="2">
         <v>3</v>
@@ -23421,10 +23421,10 @@
         <v>43047</v>
       </c>
       <c r="B641" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C641" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D641" s="2">
         <v>3</v>
@@ -23463,10 +23463,10 @@
         <v>43047</v>
       </c>
       <c r="B642" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C642" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D642" s="2">
         <v>3</v>
@@ -23505,10 +23505,10 @@
         <v>43047</v>
       </c>
       <c r="B643" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C643" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D643" s="2">
         <v>3</v>
@@ -23547,10 +23547,10 @@
         <v>43047</v>
       </c>
       <c r="B644" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C644" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D644" s="2">
         <v>3</v>
@@ -23589,10 +23589,10 @@
         <v>43047</v>
       </c>
       <c r="B645" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C645" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D645" s="2">
         <v>3</v>
@@ -23628,10 +23628,10 @@
         <v>43047</v>
       </c>
       <c r="B646" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C646" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D646" s="2">
         <v>3</v>
@@ -23661,10 +23661,10 @@
         <v>43047</v>
       </c>
       <c r="B647" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C647" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D647" s="2">
         <v>3</v>
@@ -23696,10 +23696,10 @@
         <v>43047</v>
       </c>
       <c r="B648" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C648" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D648" s="2">
         <v>3</v>
@@ -23741,10 +23741,10 @@
         <v>43047</v>
       </c>
       <c r="B649" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C649" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D649" s="2">
         <v>3</v>
@@ -23768,10 +23768,10 @@
         <v>43047</v>
       </c>
       <c r="B650" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C650" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D650" s="2">
         <v>3</v>
@@ -23800,10 +23800,10 @@
         <v>43046</v>
       </c>
       <c r="B651" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C651" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D651" s="2">
         <v>1</v>
@@ -23842,10 +23842,10 @@
         <v>43046</v>
       </c>
       <c r="B652" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C652" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D652" s="2">
         <v>1</v>
@@ -23884,10 +23884,10 @@
         <v>43046</v>
       </c>
       <c r="B653" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C653" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D653" s="2">
         <v>1</v>
@@ -23920,10 +23920,10 @@
         <v>43046</v>
       </c>
       <c r="B654" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C654" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D654" s="2">
         <v>1</v>
@@ -23947,10 +23947,10 @@
         <v>43046</v>
       </c>
       <c r="B655" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C655" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D655" s="2">
         <v>1</v>
@@ -23974,10 +23974,10 @@
         <v>43046</v>
       </c>
       <c r="B656" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C656" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D656" s="2">
         <v>1</v>
@@ -24010,10 +24010,10 @@
         <v>43046</v>
       </c>
       <c r="B657" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C657" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D657" s="2">
         <v>1</v>
@@ -24037,10 +24037,10 @@
         <v>43046</v>
       </c>
       <c r="B658" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C658" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D658" s="2">
         <v>1</v>
@@ -24064,10 +24064,10 @@
         <v>43046</v>
       </c>
       <c r="B659" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C659" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D659" s="2">
         <v>1</v>
@@ -24091,10 +24091,10 @@
         <v>43046</v>
       </c>
       <c r="B660" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C660" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D660" s="2">
         <v>1</v>
@@ -24118,10 +24118,10 @@
         <v>43046</v>
       </c>
       <c r="B661" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C661" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D661" s="2">
         <v>1</v>
@@ -24160,10 +24160,10 @@
         <v>43046</v>
       </c>
       <c r="B662" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C662" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D662" s="2">
         <v>1</v>
@@ -24196,10 +24196,10 @@
         <v>43046</v>
       </c>
       <c r="B663" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C663" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D663" s="2">
         <v>1</v>
@@ -24243,10 +24243,10 @@
         <v>43046</v>
       </c>
       <c r="B664" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C664" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D664" s="2">
         <v>1</v>
@@ -24285,10 +24285,10 @@
         <v>43046</v>
       </c>
       <c r="B665" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C665" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D665" s="2">
         <v>1</v>
@@ -24327,10 +24327,10 @@
         <v>43046</v>
       </c>
       <c r="B666" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C666" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D666" s="2">
         <v>1</v>
@@ -24354,10 +24354,10 @@
         <v>43046</v>
       </c>
       <c r="B667" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C667" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D667" s="2">
         <v>1</v>
@@ -24381,10 +24381,10 @@
         <v>43046</v>
       </c>
       <c r="B668" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C668" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D668" s="2">
         <v>2</v>
@@ -24429,10 +24429,10 @@
         <v>43046</v>
       </c>
       <c r="B669" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C669" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D669" s="2">
         <v>2</v>
@@ -24471,10 +24471,10 @@
         <v>43046</v>
       </c>
       <c r="B670" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C670" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D670" s="2">
         <v>2</v>
@@ -24513,10 +24513,10 @@
         <v>43046</v>
       </c>
       <c r="B671" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C671" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D671" s="2">
         <v>2</v>
@@ -24554,10 +24554,10 @@
         <v>43046</v>
       </c>
       <c r="B672" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C672" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D672" s="2">
         <v>2</v>
@@ -24596,10 +24596,10 @@
         <v>43046</v>
       </c>
       <c r="B673" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C673" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D673" s="2">
         <v>2</v>
@@ -24626,10 +24626,10 @@
         <v>43046</v>
       </c>
       <c r="B674" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C674" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D674" s="2">
         <v>2</v>
@@ -24668,10 +24668,10 @@
         <v>43046</v>
       </c>
       <c r="B675" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C675" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D675" s="2">
         <v>2</v>
@@ -24701,10 +24701,10 @@
         <v>43046</v>
       </c>
       <c r="B676" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C676" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D676" s="2">
         <v>2</v>
@@ -24743,10 +24743,10 @@
         <v>43046</v>
       </c>
       <c r="B677" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C677" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D677" s="2">
         <v>2</v>
@@ -24779,10 +24779,10 @@
         <v>43046</v>
       </c>
       <c r="B678" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C678" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D678" s="2">
         <v>3</v>
@@ -24827,10 +24827,10 @@
         <v>43046</v>
       </c>
       <c r="B679" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C679" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D679" s="2">
         <v>3</v>
@@ -24860,10 +24860,10 @@
         <v>43046</v>
       </c>
       <c r="B680" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C680" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D680" s="2">
         <v>3</v>
@@ -24907,10 +24907,10 @@
         <v>43046</v>
       </c>
       <c r="B681" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C681" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D681" s="2">
         <v>3</v>
@@ -24940,10 +24940,10 @@
         <v>43046</v>
       </c>
       <c r="B682" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C682" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D682" s="2">
         <v>3</v>
@@ -24985,10 +24985,10 @@
         <v>43046</v>
       </c>
       <c r="B683" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C683" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D683" s="2">
         <v>3</v>
@@ -25018,10 +25018,10 @@
         <v>43046</v>
       </c>
       <c r="B684" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C684" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D684" s="2">
         <v>3</v>
@@ -25062,10 +25062,10 @@
         <v>43046</v>
       </c>
       <c r="B685" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C685" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D685" s="2">
         <v>3</v>
@@ -25107,10 +25107,10 @@
         <v>43046</v>
       </c>
       <c r="B686" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C686" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D686" s="2">
         <v>3</v>
@@ -25151,10 +25151,10 @@
         <v>43046</v>
       </c>
       <c r="B687" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C687" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D687" s="2">
         <v>3</v>
@@ -25178,10 +25178,10 @@
         <v>43046</v>
       </c>
       <c r="B688" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C688" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D688" s="2">
         <v>1</v>
@@ -25226,10 +25226,10 @@
         <v>43046</v>
       </c>
       <c r="B689" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C689" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D689" s="2">
         <v>1</v>
@@ -25268,10 +25268,10 @@
         <v>43046</v>
       </c>
       <c r="B690" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C690" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D690" s="2">
         <v>1</v>
@@ -25310,10 +25310,10 @@
         <v>43046</v>
       </c>
       <c r="B691" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C691" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D691" s="2">
         <v>1</v>
@@ -25352,10 +25352,10 @@
         <v>43046</v>
       </c>
       <c r="B692" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C692" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D692" s="2">
         <v>1</v>
@@ -25400,10 +25400,10 @@
         <v>43046</v>
       </c>
       <c r="B693" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C693" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D693" s="2">
         <v>1</v>
@@ -25442,10 +25442,10 @@
         <v>43046</v>
       </c>
       <c r="B694" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C694" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D694" s="2">
         <v>1</v>
@@ -25487,10 +25487,10 @@
         <v>43046</v>
       </c>
       <c r="B695" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C695" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D695" s="2">
         <v>1</v>
@@ -25522,10 +25522,10 @@
         <v>43046</v>
       </c>
       <c r="B696" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C696" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D696" s="2">
         <v>2</v>
@@ -25570,10 +25570,10 @@
         <v>43046</v>
       </c>
       <c r="B697" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C697" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D697" s="2">
         <v>2</v>
@@ -25612,10 +25612,10 @@
         <v>43046</v>
       </c>
       <c r="B698" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C698" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D698" s="2">
         <v>2</v>
@@ -25645,10 +25645,10 @@
         <v>43046</v>
       </c>
       <c r="B699" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C699" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D699" s="2">
         <v>2</v>
@@ -25689,10 +25689,10 @@
         <v>43046</v>
       </c>
       <c r="B700" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C700" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D700" s="2">
         <v>2</v>
@@ -25722,10 +25722,10 @@
         <v>43046</v>
       </c>
       <c r="B701" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C701" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D701" s="2">
         <v>2</v>
@@ -25773,10 +25773,10 @@
         <v>43046</v>
       </c>
       <c r="B702" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C702" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D702" s="2">
         <v>2</v>
@@ -25812,10 +25812,10 @@
         <v>43046</v>
       </c>
       <c r="B703" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C703" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D703" s="2">
         <v>2</v>
@@ -25854,10 +25854,10 @@
         <v>43046</v>
       </c>
       <c r="B704" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C704" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D704" s="2">
         <v>2</v>
@@ -25890,10 +25890,10 @@
         <v>43046</v>
       </c>
       <c r="B705" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C705" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D705" s="2">
         <v>2</v>
@@ -25920,10 +25920,10 @@
         <v>43046</v>
       </c>
       <c r="B706" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C706" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D706" s="2">
         <v>3</v>
@@ -25959,10 +25959,10 @@
         <v>43046</v>
       </c>
       <c r="B707" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C707" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D707" s="2">
         <v>3</v>
@@ -26013,10 +26013,10 @@
         <v>43046</v>
       </c>
       <c r="B708" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C708" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D708" s="2">
         <v>3</v>
@@ -26043,10 +26043,10 @@
         <v>43046</v>
       </c>
       <c r="B709" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C709" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D709" s="2">
         <v>3</v>
@@ -26073,10 +26073,10 @@
         <v>43046</v>
       </c>
       <c r="B710" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C710" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D710" s="2">
         <v>3</v>
@@ -26106,10 +26106,10 @@
         <v>43046</v>
       </c>
       <c r="B711" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C711" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D711" s="2">
         <v>3</v>
@@ -26136,10 +26136,10 @@
         <v>43046</v>
       </c>
       <c r="B712" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C712" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D712" s="2">
         <v>3</v>
@@ -26163,10 +26163,10 @@
         <v>43046</v>
       </c>
       <c r="B713" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C713" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D713" s="2">
         <v>3</v>
@@ -26190,10 +26190,10 @@
         <v>43046</v>
       </c>
       <c r="B714" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C714" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D714" s="2">
         <v>3</v>
@@ -26232,10 +26232,10 @@
         <v>43046</v>
       </c>
       <c r="B715" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C715" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D715" s="2">
         <v>3</v>
@@ -26262,10 +26262,10 @@
         <v>43046</v>
       </c>
       <c r="B716" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C716" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D716" s="2">
         <v>3</v>
@@ -26304,10 +26304,10 @@
         <v>43046</v>
       </c>
       <c r="B717" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C717" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D717" s="2">
         <v>3</v>
@@ -26346,10 +26346,10 @@
         <v>43046</v>
       </c>
       <c r="B718" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C718" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D718" s="2">
         <v>3</v>
@@ -26385,10 +26385,10 @@
         <v>43046</v>
       </c>
       <c r="B719" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C719" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D719" s="2">
         <v>3</v>
@@ -26420,10 +26420,10 @@
         <v>43046</v>
       </c>
       <c r="B720" t="s">
+        <v>35</v>
+      </c>
+      <c r="C720" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C720" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D720" s="2">
         <v>1</v>
@@ -26462,10 +26462,10 @@
         <v>43046</v>
       </c>
       <c r="B721" t="s">
+        <v>35</v>
+      </c>
+      <c r="C721" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C721" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D721" s="2">
         <v>1</v>
@@ -26504,10 +26504,10 @@
         <v>43046</v>
       </c>
       <c r="B722" t="s">
+        <v>35</v>
+      </c>
+      <c r="C722" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C722" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D722" s="2">
         <v>1</v>
@@ -26546,10 +26546,10 @@
         <v>43046</v>
       </c>
       <c r="B723" t="s">
+        <v>35</v>
+      </c>
+      <c r="C723" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C723" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D723" s="2">
         <v>1</v>
@@ -26582,10 +26582,10 @@
         <v>43046</v>
       </c>
       <c r="B724" t="s">
+        <v>35</v>
+      </c>
+      <c r="C724" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C724" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D724" s="2">
         <v>1</v>
@@ -26618,10 +26618,10 @@
         <v>43046</v>
       </c>
       <c r="B725" t="s">
+        <v>35</v>
+      </c>
+      <c r="C725" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C725" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D725" s="2">
         <v>1</v>
@@ -26645,10 +26645,10 @@
         <v>43046</v>
       </c>
       <c r="B726" t="s">
+        <v>35</v>
+      </c>
+      <c r="C726" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C726" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D726" s="2">
         <v>1</v>
@@ -26687,10 +26687,10 @@
         <v>43046</v>
       </c>
       <c r="B727" t="s">
+        <v>35</v>
+      </c>
+      <c r="C727" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C727" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D727" s="2">
         <v>1</v>
@@ -26714,10 +26714,10 @@
         <v>43046</v>
       </c>
       <c r="B728" t="s">
+        <v>35</v>
+      </c>
+      <c r="C728" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C728" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D728" s="2">
         <v>1</v>
@@ -26756,10 +26756,10 @@
         <v>43046</v>
       </c>
       <c r="B729" t="s">
+        <v>35</v>
+      </c>
+      <c r="C729" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C729" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D729" s="2">
         <v>1</v>
@@ -26786,10 +26786,10 @@
         <v>43046</v>
       </c>
       <c r="B730" t="s">
+        <v>35</v>
+      </c>
+      <c r="C730" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C730" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D730" s="2">
         <v>1</v>
@@ -26828,10 +26828,10 @@
         <v>43046</v>
       </c>
       <c r="B731" t="s">
+        <v>35</v>
+      </c>
+      <c r="C731" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C731" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D731" s="2">
         <v>1</v>
@@ -26858,10 +26858,10 @@
         <v>43046</v>
       </c>
       <c r="B732" t="s">
+        <v>35</v>
+      </c>
+      <c r="C732" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C732" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D732" s="2">
         <v>2</v>
@@ -26900,10 +26900,10 @@
         <v>43046</v>
       </c>
       <c r="B733" t="s">
+        <v>35</v>
+      </c>
+      <c r="C733" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C733" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D733" s="2">
         <v>2</v>
@@ -26942,10 +26942,10 @@
         <v>43046</v>
       </c>
       <c r="B734" t="s">
+        <v>35</v>
+      </c>
+      <c r="C734" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C734" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D734" s="2">
         <v>2</v>
@@ -26969,10 +26969,10 @@
         <v>43046</v>
       </c>
       <c r="B735" t="s">
+        <v>35</v>
+      </c>
+      <c r="C735" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C735" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D735" s="2">
         <v>2</v>
@@ -27014,10 +27014,10 @@
         <v>43046</v>
       </c>
       <c r="B736" t="s">
+        <v>35</v>
+      </c>
+      <c r="C736" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C736" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D736" s="2">
         <v>2</v>
@@ -27041,10 +27041,10 @@
         <v>43046</v>
       </c>
       <c r="B737" t="s">
+        <v>35</v>
+      </c>
+      <c r="C737" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C737" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D737" s="2">
         <v>2</v>
@@ -27083,10 +27083,10 @@
         <v>43046</v>
       </c>
       <c r="B738" t="s">
+        <v>35</v>
+      </c>
+      <c r="C738" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C738" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D738" s="2">
         <v>2</v>
@@ -27110,10 +27110,10 @@
         <v>43046</v>
       </c>
       <c r="B739" t="s">
+        <v>35</v>
+      </c>
+      <c r="C739" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C739" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D739" s="2">
         <v>2</v>
@@ -27143,10 +27143,10 @@
         <v>43046</v>
       </c>
       <c r="B740" t="s">
+        <v>35</v>
+      </c>
+      <c r="C740" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C740" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D740" s="2">
         <v>2</v>
@@ -27187,10 +27187,10 @@
         <v>43046</v>
       </c>
       <c r="B741" t="s">
+        <v>35</v>
+      </c>
+      <c r="C741" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C741" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D741" s="2">
         <v>2</v>
@@ -27214,10 +27214,10 @@
         <v>43046</v>
       </c>
       <c r="B742" t="s">
+        <v>35</v>
+      </c>
+      <c r="C742" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C742" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D742" s="2">
         <v>2</v>
@@ -27253,10 +27253,10 @@
         <v>43046</v>
       </c>
       <c r="B743" t="s">
+        <v>35</v>
+      </c>
+      <c r="C743" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C743" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D743" s="2">
         <v>2</v>
@@ -27289,10 +27289,10 @@
         <v>43046</v>
       </c>
       <c r="B744" t="s">
+        <v>35</v>
+      </c>
+      <c r="C744" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C744" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D744" s="2">
         <v>2</v>
@@ -27324,10 +27324,10 @@
         <v>43046</v>
       </c>
       <c r="B745" t="s">
+        <v>35</v>
+      </c>
+      <c r="C745" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C745" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D745" s="2">
         <v>2</v>
@@ -27353,10 +27353,10 @@
         <v>43046</v>
       </c>
       <c r="B746" t="s">
+        <v>35</v>
+      </c>
+      <c r="C746" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C746" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D746" s="2">
         <v>3</v>
@@ -27383,10 +27383,10 @@
         <v>43046</v>
       </c>
       <c r="B747" t="s">
+        <v>35</v>
+      </c>
+      <c r="C747" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C747" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D747" s="2">
         <v>3</v>
@@ -27425,10 +27425,10 @@
         <v>43046</v>
       </c>
       <c r="B748" t="s">
+        <v>35</v>
+      </c>
+      <c r="C748" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C748" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D748" s="2">
         <v>3</v>
@@ -27467,10 +27467,10 @@
         <v>43046</v>
       </c>
       <c r="B749" t="s">
+        <v>35</v>
+      </c>
+      <c r="C749" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C749" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D749" s="2">
         <v>3</v>
@@ -27511,10 +27511,10 @@
         <v>43046</v>
       </c>
       <c r="B750" t="s">
+        <v>35</v>
+      </c>
+      <c r="C750" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C750" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D750" s="2">
         <v>3</v>
@@ -27550,10 +27550,10 @@
         <v>43046</v>
       </c>
       <c r="B751" t="s">
+        <v>35</v>
+      </c>
+      <c r="C751" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C751" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D751" s="2">
         <v>3</v>
@@ -27583,10 +27583,10 @@
         <v>43046</v>
       </c>
       <c r="B752" t="s">
+        <v>35</v>
+      </c>
+      <c r="C752" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C752" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D752" s="2">
         <v>3</v>
@@ -27625,10 +27625,10 @@
         <v>43046</v>
       </c>
       <c r="B753" t="s">
+        <v>35</v>
+      </c>
+      <c r="C753" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C753" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D753" s="2">
         <v>3</v>
@@ -27670,10 +27670,10 @@
         <v>43046</v>
       </c>
       <c r="B754" t="s">
+        <v>35</v>
+      </c>
+      <c r="C754" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C754" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D754" s="2">
         <v>3</v>
@@ -27703,10 +27703,10 @@
         <v>43046</v>
       </c>
       <c r="B755" t="s">
+        <v>35</v>
+      </c>
+      <c r="C755" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C755" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="D755" s="2">
         <v>3</v>
@@ -27745,10 +27745,10 @@
         <v>43045</v>
       </c>
       <c r="B756" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C756" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D756" s="2">
         <v>1</v>
@@ -27787,10 +27787,10 @@
         <v>43045</v>
       </c>
       <c r="B757" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C757" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D757" s="2">
         <v>1</v>
@@ -27820,10 +27820,10 @@
         <v>43045</v>
       </c>
       <c r="B758" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C758" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D758" s="2">
         <v>1</v>
@@ -27862,10 +27862,10 @@
         <v>43045</v>
       </c>
       <c r="B759" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C759" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D759" s="2">
         <v>1</v>
@@ -27901,10 +27901,10 @@
         <v>43045</v>
       </c>
       <c r="B760" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C760" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D760" s="2">
         <v>1</v>
@@ -27943,10 +27943,10 @@
         <v>43045</v>
       </c>
       <c r="B761" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C761" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D761" s="2">
         <v>1</v>
@@ -27979,10 +27979,10 @@
         <v>43045</v>
       </c>
       <c r="B762" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C762" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D762" s="2">
         <v>1</v>
@@ -28006,10 +28006,10 @@
         <v>43045</v>
       </c>
       <c r="B763" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C763" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D763" s="2">
         <v>1</v>
@@ -28048,10 +28048,10 @@
         <v>43045</v>
       </c>
       <c r="B764" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C764" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D764" s="2">
         <v>1</v>
@@ -28075,10 +28075,10 @@
         <v>43045</v>
       </c>
       <c r="B765" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C765" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D765" s="2">
         <v>1</v>
@@ -28114,10 +28114,10 @@
         <v>43045</v>
       </c>
       <c r="B766" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C766" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D766" s="2">
         <v>1</v>
@@ -28158,10 +28158,10 @@
         <v>43045</v>
       </c>
       <c r="B767" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C767" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D767" s="2">
         <v>1</v>
@@ -28185,10 +28185,10 @@
         <v>43045</v>
       </c>
       <c r="B768" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C768" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D768" s="2">
         <v>2</v>
@@ -28212,10 +28212,10 @@
         <v>43045</v>
       </c>
       <c r="B769" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C769" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D769" s="2">
         <v>2</v>
@@ -28254,10 +28254,10 @@
         <v>43045</v>
       </c>
       <c r="B770" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C770" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D770" s="2">
         <v>2</v>
@@ -28287,10 +28287,10 @@
         <v>43045</v>
       </c>
       <c r="B771" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C771" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D771" s="2">
         <v>2</v>
@@ -28332,10 +28332,10 @@
         <v>43045</v>
       </c>
       <c r="B772" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C772" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D772" s="2">
         <v>2</v>
@@ -28374,10 +28374,10 @@
         <v>43045</v>
       </c>
       <c r="B773" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C773" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D773" s="2">
         <v>2</v>
@@ -28416,10 +28416,10 @@
         <v>43045</v>
       </c>
       <c r="B774" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C774" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D774" s="2">
         <v>2</v>
@@ -28452,10 +28452,10 @@
         <v>43045</v>
       </c>
       <c r="B775" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C775" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D775" s="2">
         <v>2</v>
@@ -28502,10 +28502,10 @@
         <v>43045</v>
       </c>
       <c r="B776" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C776" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D776" s="2">
         <v>2</v>
@@ -28544,10 +28544,10 @@
         <v>43045</v>
       </c>
       <c r="B777" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C777" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D777" s="2">
         <v>2</v>
@@ -28586,10 +28586,10 @@
         <v>43045</v>
       </c>
       <c r="B778" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C778" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D778" s="2">
         <v>3</v>
@@ -28628,10 +28628,10 @@
         <v>43045</v>
       </c>
       <c r="B779" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C779" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D779" s="2">
         <v>3</v>
@@ -28670,10 +28670,10 @@
         <v>43045</v>
       </c>
       <c r="B780" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C780" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D780" s="2">
         <v>3</v>
@@ -28712,10 +28712,10 @@
         <v>43045</v>
       </c>
       <c r="B781" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C781" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D781" s="2">
         <v>3</v>
@@ -28742,10 +28742,10 @@
         <v>43045</v>
       </c>
       <c r="B782" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C782" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D782" s="2">
         <v>3</v>
@@ -28769,10 +28769,10 @@
         <v>43045</v>
       </c>
       <c r="B783" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C783" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D783" s="2">
         <v>3</v>
@@ -28808,10 +28808,10 @@
         <v>43045</v>
       </c>
       <c r="B784" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C784" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D784" s="2">
         <v>3</v>
@@ -28855,10 +28855,10 @@
         <v>43045</v>
       </c>
       <c r="B785" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C785" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D785" s="2">
         <v>3</v>
@@ -28897,10 +28897,10 @@
         <v>43045</v>
       </c>
       <c r="B786" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C786" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D786" s="2">
         <v>3</v>
@@ -28939,10 +28939,10 @@
         <v>43045</v>
       </c>
       <c r="B787" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C787" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D787" s="2">
         <v>3</v>
@@ -28981,10 +28981,10 @@
         <v>43045</v>
       </c>
       <c r="B788" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C788" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D788" s="2">
         <v>3</v>

</xml_diff>